<commit_message>
Added VisualAITests - V1
</commit_message>
<xml_diff>
--- a/LoginCredentials.xlsx
+++ b/LoginCredentials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DWork\Applitools\Hackathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2E4706-4632-418C-8A8A-1C00D61FF5CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05E7228-CA73-4F84-92B2-6D4C3DE4D732}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3396" yWindow="2964" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>userName</t>
   </si>
@@ -38,6 +38,21 @@
   </si>
   <si>
     <t>credentials</t>
+  </si>
+  <si>
+    <t>testName</t>
+  </si>
+  <si>
+    <t>UserName Password Empty</t>
+  </si>
+  <si>
+    <t>Password Empty</t>
+  </si>
+  <si>
+    <t>UserName Empty</t>
+  </si>
+  <si>
+    <t>UserName Password Exist</t>
   </si>
 </sst>
 </file>
@@ -128,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -154,6 +169,7 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,10 +495,11 @@
     <col min="1" max="1" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="3"/>
+    <col min="4" max="4" width="23.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -492,22 +509,31 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="5"/>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -515,8 +541,11 @@
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
@@ -526,30 +555,33 @@
       <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" s="9"/>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" s="9"/>
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="5"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>